<commit_message>
Moved the development commands. Put new backup files in palce.
</commit_message>
<xml_diff>
--- a/resources/data-imports/class-specials.xlsx
+++ b/resources/data-imports/class-specials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="222">
   <si>
     <t>id</t>
   </si>
@@ -627,6 +627,60 @@
   </si>
   <si>
     <t>You drink and drink and cannot seem to quench the thirst, you cannot seem to quiet the demons in your head. (Deal 80,000 Damage, growing by 8,000 damage for an additional 80,000 damage and use 40% of your damage stat towards the damage)</t>
+  </si>
+  <si>
+    <t>Merchants Coin</t>
+  </si>
+  <si>
+    <t>Merchants need their coin, don't let anyone get in the way of that!</t>
+  </si>
+  <si>
+    <t>Merchants Sale</t>
+  </si>
+  <si>
+    <t>What do you have for sale? Deals 1000 Damage growing by 10 over time for an additional 1000 damage using 5% of your damage stat.</t>
+  </si>
+  <si>
+    <t>Merchants Charm</t>
+  </si>
+  <si>
+    <t>Charm the enemy into letting their guard down. (Reduces enemy skills and resistances)</t>
+  </si>
+  <si>
+    <t>Sales Pitch</t>
+  </si>
+  <si>
+    <t>Make a sale to your enemy. They will do less damage now - through their affixes, but they might still kill you.</t>
+  </si>
+  <si>
+    <t>Caravans War</t>
+  </si>
+  <si>
+    <t>Lash out at the enemy with a caravans strength. Deal 10,000 Damage ground by 100 for an additional 10,000 damage. Use 25% of your damage stat.</t>
+  </si>
+  <si>
+    <t>Merchants Defence</t>
+  </si>
+  <si>
+    <t>Defend your self child, the enemy comes! Deals 5,000 damage growing by 50 for an additional 5,000 damage over time using 15% of your damage but only when using defend.</t>
+  </si>
+  <si>
+    <t>Coin Flip</t>
+  </si>
+  <si>
+    <t>Flip a coin and see what happens. Deals 25,000 damage growing by 250 over time for an additional 25,000 damage using 30% of your damage stat,</t>
+  </si>
+  <si>
+    <t>Caravans Last Stand</t>
+  </si>
+  <si>
+    <t>traveling with a caravan of merchants allows you to call on them when you need them the most. Deals 50,000 damage growing by 500 over time, using 15% of your damage stat. This only works when defending.</t>
+  </si>
+  <si>
+    <t>Magical Trade</t>
+  </si>
+  <si>
+    <t>Your dealings with the mages and the magical folk on the road have trained you well. Use your cast and attack to deal 60,000 damage growing by 600 over time for an additional 60,000 damage using 10% of your damage stat., The enemies spells are useless against you.</t>
   </si>
 </sst>
 </file>
@@ -962,7 +1016,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:T90"/>
+  <dimension ref="A1:T99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -3665,6 +3719,369 @@
         <v>55</v>
       </c>
     </row>
+    <row r="91" spans="1:20">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>11</v>
+      </c>
+      <c r="C91" t="s">
+        <v>204</v>
+      </c>
+      <c r="D91" t="s">
+        <v>205</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="I91">
+        <v>0.05</v>
+      </c>
+      <c r="J91">
+        <v>0.02</v>
+      </c>
+      <c r="N91">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>11</v>
+      </c>
+      <c r="C92" t="s">
+        <v>206</v>
+      </c>
+      <c r="D92" t="s">
+        <v>207</v>
+      </c>
+      <c r="E92">
+        <v>12</v>
+      </c>
+      <c r="F92">
+        <v>1000</v>
+      </c>
+      <c r="G92">
+        <v>10</v>
+      </c>
+      <c r="H92">
+        <v>0.05</v>
+      </c>
+      <c r="I92">
+        <v>0.08</v>
+      </c>
+      <c r="N92">
+        <v>0.1</v>
+      </c>
+      <c r="O92" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>11</v>
+      </c>
+      <c r="C93" t="s">
+        <v>208</v>
+      </c>
+      <c r="D93" t="s">
+        <v>209</v>
+      </c>
+      <c r="E93">
+        <v>24</v>
+      </c>
+      <c r="S93">
+        <v>0.15</v>
+      </c>
+      <c r="T93">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>11</v>
+      </c>
+      <c r="C94" t="s">
+        <v>210</v>
+      </c>
+      <c r="D94" t="s">
+        <v>211</v>
+      </c>
+      <c r="E94">
+        <v>36</v>
+      </c>
+      <c r="Q94">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>11</v>
+      </c>
+      <c r="C95" t="s">
+        <v>212</v>
+      </c>
+      <c r="D95" t="s">
+        <v>213</v>
+      </c>
+      <c r="E95">
+        <v>48</v>
+      </c>
+      <c r="F95">
+        <v>10000</v>
+      </c>
+      <c r="G95">
+        <v>100</v>
+      </c>
+      <c r="H95">
+        <v>0.25</v>
+      </c>
+      <c r="I95">
+        <v>0.2</v>
+      </c>
+      <c r="J95">
+        <v>0.1</v>
+      </c>
+      <c r="K95">
+        <v>0.05</v>
+      </c>
+      <c r="N95">
+        <v>0.25</v>
+      </c>
+      <c r="O95" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q95">
+        <v>0.1</v>
+      </c>
+      <c r="R95">
+        <v>0.05</v>
+      </c>
+      <c r="S95">
+        <v>0.15</v>
+      </c>
+      <c r="T95">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>11</v>
+      </c>
+      <c r="C96" t="s">
+        <v>214</v>
+      </c>
+      <c r="D96" t="s">
+        <v>215</v>
+      </c>
+      <c r="E96">
+        <v>60</v>
+      </c>
+      <c r="F96">
+        <v>5000</v>
+      </c>
+      <c r="G96">
+        <v>50</v>
+      </c>
+      <c r="H96">
+        <v>0.15</v>
+      </c>
+      <c r="I96">
+        <v>0.3</v>
+      </c>
+      <c r="J96">
+        <v>0.25</v>
+      </c>
+      <c r="K96">
+        <v>0.1</v>
+      </c>
+      <c r="M96">
+        <v>0.5</v>
+      </c>
+      <c r="N96">
+        <v>0.1</v>
+      </c>
+      <c r="O96" t="s">
+        <v>42</v>
+      </c>
+      <c r="P96">
+        <v>0.1</v>
+      </c>
+      <c r="Q96">
+        <v>0.2</v>
+      </c>
+      <c r="R96">
+        <v>0.1</v>
+      </c>
+      <c r="S96">
+        <v>0.1</v>
+      </c>
+      <c r="T96">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>11</v>
+      </c>
+      <c r="C97" t="s">
+        <v>216</v>
+      </c>
+      <c r="D97" t="s">
+        <v>217</v>
+      </c>
+      <c r="E97">
+        <v>70</v>
+      </c>
+      <c r="F97">
+        <v>25000</v>
+      </c>
+      <c r="G97">
+        <v>250</v>
+      </c>
+      <c r="H97">
+        <v>0.3</v>
+      </c>
+      <c r="I97">
+        <v>0.2</v>
+      </c>
+      <c r="N97">
+        <v>0.1</v>
+      </c>
+      <c r="O97" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>11</v>
+      </c>
+      <c r="C98" t="s">
+        <v>218</v>
+      </c>
+      <c r="D98" t="s">
+        <v>219</v>
+      </c>
+      <c r="E98">
+        <v>80</v>
+      </c>
+      <c r="F98">
+        <v>50000</v>
+      </c>
+      <c r="G98">
+        <v>500</v>
+      </c>
+      <c r="H98">
+        <v>0.15</v>
+      </c>
+      <c r="I98">
+        <v>0.3</v>
+      </c>
+      <c r="J98">
+        <v>0.45</v>
+      </c>
+      <c r="K98">
+        <v>0.1</v>
+      </c>
+      <c r="M98">
+        <v>0.3</v>
+      </c>
+      <c r="N98">
+        <v>0.45</v>
+      </c>
+      <c r="O98" t="s">
+        <v>42</v>
+      </c>
+      <c r="P98">
+        <v>0.25</v>
+      </c>
+      <c r="Q98">
+        <v>0.25</v>
+      </c>
+      <c r="R98">
+        <v>0.25</v>
+      </c>
+      <c r="S98">
+        <v>0.25</v>
+      </c>
+      <c r="T98">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>11</v>
+      </c>
+      <c r="C99" t="s">
+        <v>220</v>
+      </c>
+      <c r="D99" t="s">
+        <v>221</v>
+      </c>
+      <c r="E99">
+        <v>90</v>
+      </c>
+      <c r="F99">
+        <v>60000</v>
+      </c>
+      <c r="G99">
+        <v>600</v>
+      </c>
+      <c r="H99">
+        <v>0.1</v>
+      </c>
+      <c r="I99">
+        <v>0.1</v>
+      </c>
+      <c r="L99">
+        <v>0.3</v>
+      </c>
+      <c r="N99">
+        <v>0.05</v>
+      </c>
+      <c r="O99" t="s">
+        <v>60</v>
+      </c>
+      <c r="P99">
+        <v>0.75</v>
+      </c>
+      <c r="Q99">
+        <v>0.5</v>
+      </c>
+      <c r="R99">
+        <v>0.25</v>
+      </c>
+      <c r="S99">
+        <v>0.1</v>
+      </c>
+      <c r="T99">
+        <v>0.2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding Fans to the game.
Added Gunslingers Class Specials.
</commit_message>
<xml_diff>
--- a/resources/data-imports/class-specials.xlsx
+++ b/resources/data-imports/class-specials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="258">
   <si>
     <t>id</t>
   </si>
@@ -735,6 +735,60 @@
   </si>
   <si>
     <t>Reduce all listed reductions by 100%, while dealing 100,000 Damage growing by an additional 100,000 damage over time and applying 20% of your damage stat to the damage while using ANY attack. Grow your damage by 250% over time and your base damage stat by 250% over time.</t>
+  </si>
+  <si>
+    <t>Perfect Aim</t>
+  </si>
+  <si>
+    <t>Over time increase your damage and damage stat by 100%</t>
+  </si>
+  <si>
+    <t>Silencing Shot</t>
+  </si>
+  <si>
+    <t>Over time grow your damage to +150% and prevent the enemy from using their skills by up to 100%</t>
+  </si>
+  <si>
+    <t>Shock to the system</t>
+  </si>
+  <si>
+    <t>Grow your damage to +150% and reduce the enemies resistances by 100% - over time.</t>
+  </si>
+  <si>
+    <t>Sniper Shot</t>
+  </si>
+  <si>
+    <t>Deal 5,000 Damage using 20% of your damage stat as bonus - which will then grow by 500 for an additional 5,000 damage - only while using ATTACK. You will also grow your damage by +150%</t>
+  </si>
+  <si>
+    <t>Drowning Shot</t>
+  </si>
+  <si>
+    <t>Deal 10,000 Damage growing by 1,000 for an additional 10,000 damage while applying 25% of your damage stat to the damage - only while using ATTACK. Reduce all aspects of the enemy by 100% over time.</t>
+  </si>
+  <si>
+    <t>Gunslinger's Deliverance</t>
+  </si>
+  <si>
+    <t>Deal 20,000 Damage while growing it by 2,000 for an additional 20,000 and applying 27% of your damage stat as bonus damage. Damage is only dealt while using ATTACK AND CAST. You will also grow your spell damage by 125% over time and reduce the enemies spell evasion and affix damage by 100% over time.</t>
+  </si>
+  <si>
+    <t>Devastating Blow</t>
+  </si>
+  <si>
+    <t>Deal 25,000 Damage growing by 2,500 damage for an additional 25,000 damage with 30% of your damage stat as bonus. This only procs while using ATTACK. You will also grow your own damage by +250% over time.</t>
+  </si>
+  <si>
+    <t>Spell Shot</t>
+  </si>
+  <si>
+    <t>Deal 50,000 in damage growing by 5,000 for an additional 50,000 damage while applying 12% of your damage stat as bonus damage. Damage only procs during Cast and Attack. Reduce ass aspects on an enemy by 100% over time and grow your own spell damage by +200%</t>
+  </si>
+  <si>
+    <t>Defensive Shot</t>
+  </si>
+  <si>
+    <t>Deal 75,000 Damage growing by 7,500 damage while applying 40% of your damage stat to the over all damage as a bonus. Only procs when using DEFEND. Will also grow your base damage stat by +300% overtime.</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1128,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:T108"/>
+  <dimension ref="A1:T117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -4449,6 +4503,300 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="109" spans="1:20">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>14</v>
+      </c>
+      <c r="C109" t="s">
+        <v>240</v>
+      </c>
+      <c r="D109" t="s">
+        <v>241</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="I109">
+        <v>0.01</v>
+      </c>
+      <c r="N109">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <v>14</v>
+      </c>
+      <c r="C110" t="s">
+        <v>242</v>
+      </c>
+      <c r="D110" t="s">
+        <v>243</v>
+      </c>
+      <c r="E110">
+        <v>12</v>
+      </c>
+      <c r="I110">
+        <v>0.015</v>
+      </c>
+      <c r="S110">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111">
+        <v>14</v>
+      </c>
+      <c r="C111" t="s">
+        <v>244</v>
+      </c>
+      <c r="D111" t="s">
+        <v>245</v>
+      </c>
+      <c r="E111">
+        <v>24</v>
+      </c>
+      <c r="N111">
+        <v>0.015</v>
+      </c>
+      <c r="T111">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112">
+        <v>14</v>
+      </c>
+      <c r="C112" t="s">
+        <v>246</v>
+      </c>
+      <c r="D112" t="s">
+        <v>247</v>
+      </c>
+      <c r="E112">
+        <v>36</v>
+      </c>
+      <c r="F112">
+        <v>5000</v>
+      </c>
+      <c r="G112">
+        <v>500</v>
+      </c>
+      <c r="H112">
+        <v>0.2</v>
+      </c>
+      <c r="I112">
+        <v>0.01</v>
+      </c>
+      <c r="O112" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>14</v>
+      </c>
+      <c r="C113" t="s">
+        <v>248</v>
+      </c>
+      <c r="D113" t="s">
+        <v>249</v>
+      </c>
+      <c r="E113">
+        <v>48</v>
+      </c>
+      <c r="F113">
+        <v>10000</v>
+      </c>
+      <c r="G113">
+        <v>1000</v>
+      </c>
+      <c r="H113">
+        <v>0.25</v>
+      </c>
+      <c r="O113" t="s">
+        <v>55</v>
+      </c>
+      <c r="P113">
+        <v>0.01</v>
+      </c>
+      <c r="Q113">
+        <v>0.01</v>
+      </c>
+      <c r="R113">
+        <v>0.01</v>
+      </c>
+      <c r="S113">
+        <v>0.01</v>
+      </c>
+      <c r="T113">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114">
+        <v>14</v>
+      </c>
+      <c r="C114" t="s">
+        <v>250</v>
+      </c>
+      <c r="D114" t="s">
+        <v>251</v>
+      </c>
+      <c r="E114">
+        <v>60</v>
+      </c>
+      <c r="F114">
+        <v>20000</v>
+      </c>
+      <c r="G114">
+        <v>2000</v>
+      </c>
+      <c r="H114">
+        <v>0.27</v>
+      </c>
+      <c r="L114">
+        <v>0.012</v>
+      </c>
+      <c r="O114" t="s">
+        <v>60</v>
+      </c>
+      <c r="P114">
+        <v>0.01</v>
+      </c>
+      <c r="Q114">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115">
+        <v>14</v>
+      </c>
+      <c r="C115" t="s">
+        <v>252</v>
+      </c>
+      <c r="D115" t="s">
+        <v>253</v>
+      </c>
+      <c r="E115">
+        <v>70</v>
+      </c>
+      <c r="F115">
+        <v>25000</v>
+      </c>
+      <c r="G115">
+        <v>2500</v>
+      </c>
+      <c r="H115">
+        <v>0.3</v>
+      </c>
+      <c r="N115">
+        <v>0.025</v>
+      </c>
+      <c r="O115" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116">
+        <v>14</v>
+      </c>
+      <c r="C116" t="s">
+        <v>254</v>
+      </c>
+      <c r="D116" t="s">
+        <v>255</v>
+      </c>
+      <c r="E116">
+        <v>80</v>
+      </c>
+      <c r="F116">
+        <v>50000</v>
+      </c>
+      <c r="G116">
+        <v>5000</v>
+      </c>
+      <c r="H116">
+        <v>0.12</v>
+      </c>
+      <c r="L116">
+        <v>0.02</v>
+      </c>
+      <c r="O116" t="s">
+        <v>91</v>
+      </c>
+      <c r="P116">
+        <v>0.01</v>
+      </c>
+      <c r="Q116">
+        <v>0.01</v>
+      </c>
+      <c r="R116">
+        <v>0.01</v>
+      </c>
+      <c r="S116">
+        <v>0.01</v>
+      </c>
+      <c r="T116">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>14</v>
+      </c>
+      <c r="C117" t="s">
+        <v>256</v>
+      </c>
+      <c r="D117" t="s">
+        <v>257</v>
+      </c>
+      <c r="E117">
+        <v>90</v>
+      </c>
+      <c r="F117">
+        <v>75000</v>
+      </c>
+      <c r="G117">
+        <v>7500</v>
+      </c>
+      <c r="H117">
+        <v>0.4</v>
+      </c>
+      <c r="N117">
+        <v>0.03</v>
+      </c>
+      <c r="O117" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added support for maces.
</commit_message>
<xml_diff>
--- a/resources/data-imports/class-specials.xlsx
+++ b/resources/data-imports/class-specials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="276">
   <si>
     <t>id</t>
   </si>
@@ -758,37 +758,91 @@
     <t>Sniper Shot</t>
   </si>
   <si>
-    <t>Deal 5,000 Damage using 20% of your damage stat as bonus - which will then grow by 500 for an additional 5,000 damage - only while using ATTACK. You will also grow your damage by +150%</t>
+    <t>Deal 5,000 Damage using 20% of your damage stat as bonus - which will then grow by 50 for an additional 5,000 damage - only while using ATTACK. You will also grow your damage by +150%</t>
   </si>
   <si>
     <t>Drowning Shot</t>
   </si>
   <si>
-    <t>Deal 10,000 Damage growing by 1,000 for an additional 10,000 damage while applying 25% of your damage stat to the damage - only while using ATTACK. Reduce all aspects of the enemy by 100% over time.</t>
+    <t>Deal 10,000 Damage growing by 100 for an additional 10,000 damage while applying 25% of your damage stat to the damage - only while using ATTACK. Reduce all aspects of the enemy by 100% over time.</t>
   </si>
   <si>
     <t>Gunslinger's Deliverance</t>
   </si>
   <si>
-    <t>Deal 20,000 Damage while growing it by 2,000 for an additional 20,000 and applying 27% of your damage stat as bonus damage. Damage is only dealt while using ATTACK AND CAST. You will also grow your spell damage by 125% over time and reduce the enemies spell evasion and affix damage by 100% over time.</t>
+    <t>Deal 20,000 Damage while growing it by 200 for an additional 20,000 and applying 27% of your damage stat as bonus damage. Damage is only dealt while using ATTACK AND CAST. You will also grow your spell damage by 125% over time and reduce the enemies spell evasion and affix damage by 100% over time.</t>
   </si>
   <si>
     <t>Devastating Blow</t>
   </si>
   <si>
-    <t>Deal 25,000 Damage growing by 2,500 damage for an additional 25,000 damage with 30% of your damage stat as bonus. This only procs while using ATTACK. You will also grow your own damage by +250% over time.</t>
+    <t>Deal 25,000 Damage growing by 250 damage for an additional 25,000 damage with 30% of your damage stat as bonus. This only procs while using ATTACK. You will also grow your own damage by +250% over time.</t>
   </si>
   <si>
     <t>Spell Shot</t>
   </si>
   <si>
-    <t>Deal 50,000 in damage growing by 5,000 for an additional 50,000 damage while applying 12% of your damage stat as bonus damage. Damage only procs during Cast and Attack. Reduce ass aspects on an enemy by 100% over time and grow your own spell damage by +200%</t>
+    <t>Deal 50,000 in damage growing by 500 for an additional 50,000 damage while applying 12% of your damage stat as bonus damage. Damage only procs during Cast and Attack. Reduce ass aspects on an enemy by 100% over time and grow your own spell damage by +200%</t>
   </si>
   <si>
     <t>Defensive Shot</t>
   </si>
   <si>
-    <t>Deal 75,000 Damage growing by 7,500 damage while applying 40% of your damage stat to the over all damage as a bonus. Only procs when using DEFEND. Will also grow your base damage stat by +300% overtime.</t>
+    <t>Deal 75,000 Damage growing by 750 damage while applying 40% of your damage stat to the over all damage as a bonus. Only procs when using DEFEND. Will also grow your base damage stat by +300% overtime.</t>
+  </si>
+  <si>
+    <t>Clerical Prayer</t>
+  </si>
+  <si>
+    <t>Over time grow your health by +50% and boost your healing - done through healing spells - by +150% over time.</t>
+  </si>
+  <si>
+    <t>Churches Grace</t>
+  </si>
+  <si>
+    <t>Increase Damage, Healing and Armour class by 150% and 170% (For AC overtime. Increase your health and damage stat by 75% over time,</t>
+  </si>
+  <si>
+    <t>Blessed Rage</t>
+  </si>
+  <si>
+    <t>Reduce all aspects of the enemy (see reductions) by 100% over time. Increase your Armour class by 100%, Base Healing (through healing spells) by 170%, Spell Damage by 50%, health and damage stat by 100% - all overtime.</t>
+  </si>
+  <si>
+    <t>Faithless War Cry</t>
+  </si>
+  <si>
+    <t>Deal 5,000 damage growing by 50 for an additional 5,000 damage while applying 5% of your damage stat as bonus damage. must use ATTACK for this to proc. You will grow your damage stat by 150% over time.</t>
+  </si>
+  <si>
+    <t>Malicious Prayer</t>
+  </si>
+  <si>
+    <t>Deal 10,000 damage growing by 100 over time dealing an additional 10,000 damage, while applying 10% of your damage stat towards the damage. This will only proc while using ATTACK AND CAST. Grow your healing and damage stat by 200% over time and grow your health by 100%, overtime.</t>
+  </si>
+  <si>
+    <t>The Churches Holy Magic</t>
+  </si>
+  <si>
+    <t>Grow healing (Healing Spells) by 250%, Spell damage by 150% and your damage stat by 200% over time. Deal 25,000 damage, growing by 250 damage over time for an additional 25,000 damage., which will apply 20% of your damage stat as bonus damage - however this only procs if you use: CAST</t>
+  </si>
+  <si>
+    <t>Churches Defence</t>
+  </si>
+  <si>
+    <t>Deal 40,000 damage, growing by 400 for an additional, 40,000 damage while applying 18% of your damage stat as bonus damage. Only procs if you use DEFEND. Grow your own AC by 200% over time.</t>
+  </si>
+  <si>
+    <t>Wrath of the true God</t>
+  </si>
+  <si>
+    <t>Deal 60,000 Damage growing by 600 for an additional 60,000 damage while applying 15% of your damage stat as bonus damage. Only procs during ATTACK AND CAST. Grow your damage, ac and healing by 200% over time. Grow your damage stat by 300% over time.</t>
+  </si>
+  <si>
+    <t>Churches Blessing on the Faithless</t>
+  </si>
+  <si>
+    <t>Deal 75,000 damage growing by 750 over time while adding 10% of your damage stat as bonus damage. Will proc during ANY attack type. Will grow all your modifiers by 200% overtime - such as Damage, Healing, Spell Damage, Health and Damage Stat.</t>
   </si>
 </sst>
 </file>
@@ -1128,7 +1182,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:T117"/>
+  <dimension ref="A1:T126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1138,7 +1192,7 @@
   <cols>
     <col min="1" max="1" width="4.57" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="31.707" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="41.133" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="388.048" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="30.564" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="19.995" bestFit="true" customWidth="true" style="0"/>
@@ -4592,7 +4646,7 @@
         <v>5000</v>
       </c>
       <c r="G112">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="H112">
         <v>0.2</v>
@@ -4624,7 +4678,7 @@
         <v>10000</v>
       </c>
       <c r="G113">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="H113">
         <v>0.25</v>
@@ -4668,7 +4722,7 @@
         <v>20000</v>
       </c>
       <c r="G114">
-        <v>2000</v>
+        <v>200</v>
       </c>
       <c r="H114">
         <v>0.27</v>
@@ -4706,7 +4760,7 @@
         <v>25000</v>
       </c>
       <c r="G115">
-        <v>2500</v>
+        <v>250</v>
       </c>
       <c r="H115">
         <v>0.3</v>
@@ -4738,7 +4792,7 @@
         <v>50000</v>
       </c>
       <c r="G116">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="H116">
         <v>0.12</v>
@@ -4785,7 +4839,7 @@
         <v>75000</v>
       </c>
       <c r="G117">
-        <v>7500</v>
+        <v>750</v>
       </c>
       <c r="H117">
         <v>0.4</v>
@@ -4795,6 +4849,351 @@
       </c>
       <c r="O117" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>13</v>
+      </c>
+      <c r="C118" t="s">
+        <v>258</v>
+      </c>
+      <c r="D118" t="s">
+        <v>259</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="K118">
+        <v>0.015</v>
+      </c>
+      <c r="M118">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119">
+        <v>13</v>
+      </c>
+      <c r="C119" t="s">
+        <v>260</v>
+      </c>
+      <c r="D119" t="s">
+        <v>261</v>
+      </c>
+      <c r="E119">
+        <v>12</v>
+      </c>
+      <c r="I119">
+        <v>0.015</v>
+      </c>
+      <c r="J119">
+        <v>0.017</v>
+      </c>
+      <c r="K119">
+        <v>0.015</v>
+      </c>
+      <c r="M119">
+        <v>0.0075</v>
+      </c>
+      <c r="N119">
+        <v>0.0075</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120">
+        <v>13</v>
+      </c>
+      <c r="C120" t="s">
+        <v>262</v>
+      </c>
+      <c r="D120" t="s">
+        <v>263</v>
+      </c>
+      <c r="E120">
+        <v>24</v>
+      </c>
+      <c r="J120">
+        <v>0.01</v>
+      </c>
+      <c r="K120">
+        <v>0.017</v>
+      </c>
+      <c r="L120">
+        <v>0.005</v>
+      </c>
+      <c r="M120">
+        <v>0.01</v>
+      </c>
+      <c r="N120">
+        <v>0.01</v>
+      </c>
+      <c r="P120">
+        <v>0.01</v>
+      </c>
+      <c r="Q120">
+        <v>0.01</v>
+      </c>
+      <c r="R120">
+        <v>0.01</v>
+      </c>
+      <c r="S120">
+        <v>0.01</v>
+      </c>
+      <c r="T120">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>13</v>
+      </c>
+      <c r="C121" t="s">
+        <v>264</v>
+      </c>
+      <c r="D121" t="s">
+        <v>265</v>
+      </c>
+      <c r="E121">
+        <v>36</v>
+      </c>
+      <c r="F121">
+        <v>5000</v>
+      </c>
+      <c r="G121">
+        <v>50</v>
+      </c>
+      <c r="H121">
+        <v>0.05</v>
+      </c>
+      <c r="N121">
+        <v>0.015</v>
+      </c>
+      <c r="O121" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122">
+        <v>13</v>
+      </c>
+      <c r="C122" t="s">
+        <v>266</v>
+      </c>
+      <c r="D122" t="s">
+        <v>267</v>
+      </c>
+      <c r="E122">
+        <v>48</v>
+      </c>
+      <c r="F122">
+        <v>10000</v>
+      </c>
+      <c r="G122">
+        <v>100</v>
+      </c>
+      <c r="H122">
+        <v>0.1</v>
+      </c>
+      <c r="K122">
+        <v>0.02</v>
+      </c>
+      <c r="M122">
+        <v>0.01</v>
+      </c>
+      <c r="N122">
+        <v>0.02</v>
+      </c>
+      <c r="O122" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123">
+        <v>13</v>
+      </c>
+      <c r="C123" t="s">
+        <v>268</v>
+      </c>
+      <c r="D123" t="s">
+        <v>269</v>
+      </c>
+      <c r="E123">
+        <v>60</v>
+      </c>
+      <c r="F123">
+        <v>25000</v>
+      </c>
+      <c r="G123">
+        <v>250</v>
+      </c>
+      <c r="H123">
+        <v>0.2</v>
+      </c>
+      <c r="K123">
+        <v>0.025</v>
+      </c>
+      <c r="L123">
+        <v>0.015</v>
+      </c>
+      <c r="N123">
+        <v>0.02</v>
+      </c>
+      <c r="O123" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124">
+        <v>13</v>
+      </c>
+      <c r="C124" t="s">
+        <v>270</v>
+      </c>
+      <c r="D124" t="s">
+        <v>271</v>
+      </c>
+      <c r="E124">
+        <v>70</v>
+      </c>
+      <c r="F124">
+        <v>40000</v>
+      </c>
+      <c r="G124">
+        <v>400</v>
+      </c>
+      <c r="H124">
+        <v>0.18</v>
+      </c>
+      <c r="J124">
+        <v>0.02</v>
+      </c>
+      <c r="O124" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <v>13</v>
+      </c>
+      <c r="C125" t="s">
+        <v>272</v>
+      </c>
+      <c r="D125" t="s">
+        <v>273</v>
+      </c>
+      <c r="E125">
+        <v>80</v>
+      </c>
+      <c r="F125">
+        <v>60000</v>
+      </c>
+      <c r="G125">
+        <v>600</v>
+      </c>
+      <c r="H125">
+        <v>0.15</v>
+      </c>
+      <c r="I125">
+        <v>0.02</v>
+      </c>
+      <c r="J125">
+        <v>0.02</v>
+      </c>
+      <c r="K125">
+        <v>0.02</v>
+      </c>
+      <c r="N125">
+        <v>0.03</v>
+      </c>
+      <c r="O125" t="s">
+        <v>60</v>
+      </c>
+      <c r="P125">
+        <v>0.01</v>
+      </c>
+      <c r="Q125">
+        <v>0.01</v>
+      </c>
+      <c r="R125">
+        <v>0.01</v>
+      </c>
+      <c r="S125">
+        <v>0.01</v>
+      </c>
+      <c r="T125">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126">
+        <v>13</v>
+      </c>
+      <c r="C126" t="s">
+        <v>274</v>
+      </c>
+      <c r="D126" t="s">
+        <v>275</v>
+      </c>
+      <c r="E126">
+        <v>90</v>
+      </c>
+      <c r="F126">
+        <v>75000</v>
+      </c>
+      <c r="G126">
+        <v>750</v>
+      </c>
+      <c r="H126">
+        <v>0.1</v>
+      </c>
+      <c r="I126">
+        <v>0.02</v>
+      </c>
+      <c r="J126">
+        <v>0.02</v>
+      </c>
+      <c r="K126">
+        <v>0.02</v>
+      </c>
+      <c r="L126">
+        <v>0.02</v>
+      </c>
+      <c r="M126">
+        <v>0.02</v>
+      </c>
+      <c r="N126">
+        <v>0.02</v>
+      </c>
+      <c r="O126" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>